<commit_message>
started work on the requirements
</commit_message>
<xml_diff>
--- a/docs/Eisen.xlsx
+++ b/docs/Eisen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\WebstormProjects\fakeStore\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tynek\WebstormProjects\fakeStore\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9B049B-4D54-4CFE-B150-132F99C23F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931DA152-D0C5-4630-9562-6B1A1638EFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50FB539B-D8C3-40BF-ABB1-A5265842B59E}"/>
+    <workbookView xWindow="38280" yWindow="13275" windowWidth="29040" windowHeight="15720" xr2:uid="{50FB539B-D8C3-40BF-ABB1-A5265842B59E}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,84 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Een gebruiker moet kunnen registreren, dit kan op een registratie pagina, 
+deze is te vinden door te klikken op registreer vanuit de login pagina. </t>
+  </si>
+  <si>
+    <t>Bij het registreren moeten de wachtwoorden aan elkaar gelijk zijn en ook aan de eisen voldoen.</t>
+  </si>
+  <si>
+    <t>Zodra alle registratie informatie is ingevuld moet de gebruiker een alert krijgen op zijn scherm dat het gelukt is, vervolgens moet hij/zij door naar de Home pagina gestuurd worden.</t>
+  </si>
+  <si>
+    <t>(Private Routes) Als een gebruiker niet ingelogd is, moet elke pagina naar de login pagina omleiden met de een bericht dat de gebruiker moet inloggen om gebruik te kunnen maken van de pagina</t>
+  </si>
+  <si>
+    <t>Een gebruiker moet kunnen inloggen via de login pagina</t>
+  </si>
+  <si>
+    <t>Er moet een profiel pagina zijn die door middel van de navigatiebalk te bereiken is</t>
+  </si>
+  <si>
+    <t>Op de Profiel pagina zijn de gegevens van de gebruiker te zien, email, gebruikersnaam, en adresgegevens</t>
+  </si>
+  <si>
+    <t>De gebruiker moet op deze pagina, met behulp van een knop zijn gegevens, kunnen wijzigen. Hieronder valt zijn gebruikersnaam, zijn email, adres en zijn wachtwoord.</t>
+  </si>
+  <si>
+    <t>Er moet en Sell pagina aanwezig zijn die door middel van de navigatiebalk onder het tabje Sell te bereiken is</t>
+  </si>
+  <si>
+    <t>Er moet een products pagina zijn die door middel van de navigatiebalk onder products te vinden is</t>
+  </si>
+  <si>
+    <t>Er moet een specifieke product pagina zijn die door middel van het op het product te klikken op de producten pagina te bereiken is</t>
+  </si>
+  <si>
+    <t>Er moet een cart pagina zijn die door middel van een link op de navigatiebalk te vinden is</t>
+  </si>
+  <si>
+    <t>Voor een definitieve aanpassing der gegevens, moet er een vraag gesteld worden, de gebruiker moet Change in hoofdletters intypen en pas dan zullen de gegevens daadwerkelijk aangepast worden</t>
+  </si>
+  <si>
+    <t>Een gebruiker moet op de navigatie balk een logout knop kunnen zien, op het moment dat de gebruiker op de Logout knop klikt meot deze uitgelogd worden.</t>
+  </si>
+  <si>
+    <t>Een gebruiker moet op de navigatiebalk een theme knop te zien krijgen, op het moment dat deze geklikt wordt moet de theme updaten</t>
+  </si>
+  <si>
+    <t>Een ingelogde gebruiker die items zit te bekijken, kan een icoontje op de pagina klikken waardoor het drankje aan de mand is toegevoegd</t>
+  </si>
+  <si>
+    <t>Een gebruiker kan ook een item uit zijn cart verwijderen als deze der eenmaal in zit.</t>
+  </si>
+  <si>
+    <t>Een gebruiker moet op de products page categories aan en uit kunen vinken om zo met behulp van verschillende filters te zoeken.</t>
+  </si>
+  <si>
+    <t>Op het moment dat de er een backend request wordt gemaakt krijgen we een buffering icoontje te zien</t>
+  </si>
+  <si>
+    <t>Er is ten aller tijden een navigatie balk</t>
+  </si>
+  <si>
+    <t>Items moeten uniform en op een mooie stijlvolle manier gepresenteerd worden</t>
+  </si>
+  <si>
+    <t>Elke item heeft bij een Hover een ander gedrag als wanneer deze normaal op de pagina weergegeven wordt</t>
+  </si>
+  <si>
+    <t>Je moet op verschillende beeld afmetingen de pagina nog kunnen zien en gebruiken, op deze manier kan je dus de pagina op beide smartphones of op full-size desktop monitors gebruiken.</t>
+  </si>
+  <si>
+    <t>Als er een fout is bij het halen van een request naar de backend, wordt dit aan de gebruiker doorgegeven.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -95,15 +173,89 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -120,10 +272,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="719995"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -432,15 +584,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E3582-EACF-42CA-9681-43C1A515A0A2}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="174.21875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <v>16</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <v>18</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <v>20</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <v>22</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>23</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>24</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -451,9 +833,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continued work on the requirements
</commit_message>
<xml_diff>
--- a/docs/Eisen.xlsx
+++ b/docs/Eisen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tynek\WebstormProjects\fakeStore\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\WebstormProjects\fakeStore\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931DA152-D0C5-4630-9562-6B1A1638EFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0F06C8-0841-4DCA-B4A1-8EA1B783F362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="13275" windowWidth="29040" windowHeight="15720" xr2:uid="{50FB539B-D8C3-40BF-ABB1-A5265842B59E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50FB539B-D8C3-40BF-ABB1-A5265842B59E}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t xml:space="preserve">Een gebruiker moet kunnen registreren, dit kan op een registratie pagina, 
 deze is te vinden door te klikken op registreer vanuit de login pagina. </t>
@@ -110,6 +110,183 @@
   </si>
   <si>
     <t>Als er een fout is bij het halen van een request naar de backend, wordt dit aan de gebruiker doorgegeven.</t>
+  </si>
+  <si>
+    <t>Bij de registratie worden alle waardes aan de voorkant gecontroleerd met een if statement, als er een fout is waardoor de registratie niet voltooid kan worden, wordt er een melding gedaan, en wordt de gebruiker vervolgens terug naar het registreer scherm gestuurd met alle al ingevulde informatie.</t>
+  </si>
+  <si>
+    <t>Op het moment dat alle gebruikers gegevens correct zijn worden deze opgeslagen in een object en d.m.v. een Post request naar de backend estuurd, voortaan zal de gebruiker deze gegevens kunnen gebruiken om in te loggen</t>
+  </si>
+  <si>
+    <t>Dit wordt met behulp van een try catch blok gedaan, deze zorgt ervoor dat er een melding verschijn als er iets misgaat.</t>
+  </si>
+  <si>
+    <t>Als alles ingevuld is wordt er met behulp van routes een link getoont op de pagina, deze herleidt naar de login pagina</t>
+  </si>
+  <si>
+    <t>Als een gebruiker niet is ingelogd, dit wordt standaard door context aangegeven, dan moet elke pagina de gebruiker naar de login pagina/register pagine terugleiden, dit doen we door middel van een login required page, deze pagina roepen we aan als een component bij elke pagina als authorized context op false staat, dit kunnen we door middel van een if statement op de pagina doen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als een gebruiker gegevens invoert om in te loggen, worden deze met een POST request naar de backend gestuurd, afhankelijk daarvan krijgt de gebruiker een JSX-token, </t>
+  </si>
+  <si>
+    <t>De POST request wordt ook binnen een try catch blok geplaatst om op die manier errors die eruit komen te kunnen vermelden, op die manier kan de gebruiker kijken en reageren, stel voor zijn kat bijt de ethernet kabel door, dan weet hij wat het probleem is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We slaan de JSX-token op met behulp van een asynchrone functie en state, in een variabele genoemd loginSuccess </t>
+  </si>
+  <si>
+    <t>Als de loginSuccess variabele truthy is dan wordt de gebruiker ingelogd. anders wordt er een melding in de vorm van een alert zichtbaar, dit is mogelijk met een if else statement. Als loginSucces truthy is dan loggen we de gebruiker met behulp van state en in, op alle andere pagina’s wordt de loginSuccess state met context binnengehaald om op die manier de gebruiker te autoriseren om door te kunnen gaan. Als de gebruiker faalt met het inloggen krijgen ze nogmaals de capaciteit om te proberen in te loggen op de login pagina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> behulp van routing kunnen we op de navigatie balk een nav linken naar de profiel pagina als de gebruiker ingelogd is</t>
+  </si>
+  <si>
+    <t>data op de profiel pagina (mail, username, password) zal door middel van een Get request binnen een try catch blok gepakt worden om op de pagina getoont te worden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> er een foto is geupload door de gebruiker, dan zal deze met een andere GET request binnen een try catch blok gehaald worden en op de pagina verschijnen. Als er een GET gemaakt wordt en het antwoord is leeg, dan gebruiken state om een variabele profilePictureIsEmpty op true te zetten</t>
+  </si>
+  <si>
+    <t>de Profiel Pagina zal er een knop zijn met een label, de label is gegevens bewerken. Op het moment dat de knop gedrukt wordt zal het een handleClick functie aanroepen. Deze zal een variabele bewerkingsmodus door middel van state aanpassen naar true.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> een input van type file zullen we een foto kunnen selecteren, vervolgens zullen we een asynchrone axios functie aan kunnen roepen met een onChange event listener. Op deze manier kunnen we een profielfoto uploaden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profiel Pagina is een pagina die voor de return statement een if statement heeft, daardoor zullen we met hulp van of de ene conditie of de andere de pagina op een andere manier kunnen laten zien, waar eerder de gegevens niet te bewerken waren, zal er nu door het feit dat de bewerkingsmodus variabele nu op true staat een andere versie van de pagina te zien zijn, aangezien er nu een andere return statement aangeroepen wordt. Dit betekent dat we de gegevens nu in een form kunnen zetten, met textvelden als inputs met bijbehorende labels. </t>
+  </si>
+  <si>
+    <t>kunnen dan met een onSubmit button en vraag laten verschijnen met instructies, als de gebruiker echt wil aanpassen moet deze CHANGE intypen en vervolgens zullen we met behulp van een PUT request de gegevens naar de backend sturen. Hierna zullen de gegevens anders zijn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> er nog geen profielfoto is voor de gebruiker, zal deze een nieuwe kunnen uploaden met behulp van de upload profile picture knop, deze zal alleen te zien zijn als de variabele ProfilePictureIsEmpty true is, de gebruiker zal erop kunnen klikken, een foto selecteren uit een willekeurige directory op zijn PC, en vervolgens op upload klikken, daarna zal er een POST request met de foto naar de backend gestuurd worden, voortaan zal de foto op de profiel pagina te zien zijn.</t>
+  </si>
+  <si>
+    <t>zal een button op de navigatiebalk geplaatst worden, deze button zal een functie hebben waar er een popup te zien wordt, dit door middel van een handleClick functie wat andere content laat zien op de pagina, namelijk een popup met de vraag of de gebruiker het zeker weet of hij wil uitloggen of niet. Vervolgens kunnen we voor de logout knop die getriggered wordt indien de gebruiker op Ja klikt een handleLogout functie aanroepen, deze functie kunnen we in de context zetten en in de navigatiebalk importeren, als deze wordt aangeroepen zet de functie, de state van de isAuthorized variabele op false en kunnen we op die manier uitloggen.</t>
+  </si>
+  <si>
+    <t>elke vorm van zoeken wordt een component gebruikt om drankjes te weergeven in een standaardformaat. Dit component noemen we DrinkItem, het wordt gebruikt met vooraf bepaalde styling, afmetingen en andere belangrijke dingen. Met behulp van een klikbaar element met een CSS animation kunnen we een aanroepbare functie in het component zetten welke het ID van een drankje kan doorgeven aan een lijst van onze favorieten als deze er niet alvast in staat. Deze lijst van favorieten wordt d.m.v. een PUT request in onze gebruikers gegevens opgeslagen. Voortaan zullen deze ids van de drankjes met een GET request ook gehaald worden bij het inloggen, we zullen dus voor dat we het drank ID aan onze favorieten lijst toevoegen eerst moeten kijken of deze er alvast in staat, pas dan kunnen we hem toevoegen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ingelogde gebruiker kan zijn favorieten pagina openen indien hij op zijn favorieten klikt in de navigatie balk, dan worden zijn drankjes in een preview vorm op de pagina te zien, de dranken en hun gegevens/afbeeldingen worden nu op basis van ID met een GET request gehaald vanuit de backend en op de pagina gepresenteerd. In hetzelfde formaat als wat al in gebruik is. Het enige verschil is dat de drankjes met een ander component te zien zijn en dit component heeft een andere functie, dit component kan namelijk het drankje uit de favorieten verwijderen, de state van de favorieten die geïmporteerd is wordt dus aangepast met een array methode, en er wordt ook gelijk een PUT request gemaakt naar de backend om dit drankje te verwijderen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> behulp van state kunnen we de hoeveelheid drankjes die we willen weergeven vastleggen, we zullen er 10 per pagina laten zien, we zullen ook de mogelijkheid hebben om door te bladeren en een pagina terug te gaan met behulp van state, deze zal met last 10 en next 10 gedaan kunnen worden.</t>
+  </si>
+  <si>
+    <t>nav bar heeft een nav/route naar de categorieën pagina, op deze manier kunnen we deze pagina bereiken</t>
+  </si>
+  <si>
+    <t>het moment dat de nav categorieën geklikt wordt, halen we met een asynchrone axios GET request van de backend de hele lijst aan categorieën binnen, deze slaan we op in een categorieën variabele.</t>
+  </si>
+  <si>
+    <t>hebben alvast componenten gemaakt waarin we de namen van elke categorie kunnen tonen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> een map methode itereren we door de categorieën array die we uit de backend gepakt hebben, we zetten elke individuele categorieën entry op de pagina indien we het met de map methode als prop doorgeven aan het categorie component wat alvast gemaakt is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> component wat telkens een Categorie naam op de pagina weergeeft, heeft een onClick attribuut, dit attribuut roept een handleCategoryChoice functie aan die we alvast gedefinieerd hebben</t>
+  </si>
+  <si>
+    <t>alvast gemaakte handleCategoryChoice functie is in de component gedefinieerd en heeft dus ook al de capaciteit om binnen de scope van het component een property mee te krijgen</t>
+  </si>
+  <si>
+    <t>handleCategoryChoice heeft een nav, de gebruiker wordt herleid naar de searchByCategories page, dit wordt gedaan met de Route waar de naam van de categorie alvast aan de path geconcateneerd is, deze geconcateneerde string wordt gebruikt in een axios asynch GET request naar de Cocktail DB backend en haalt vervolgens data op uit de backend. Deze data slaan we op in een variabele namens results.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> behulp van state en een beperkte hoeveelheid die we binnen halen kunnen we de paginas vullen, met een vooraf bepaalde hoeveelheid entries.</t>
+  </si>
+  <si>
+    <t>beginnende hoeveelheid entries per pagina is 10. Daarmee kunnen we de volgende 10 of de laatste 10 (als we eenmaal geklikt hebben) ophalen met een axios GET request en vervolgens gebruik van state.</t>
+  </si>
+  <si>
+    <t>hoeveelheid drankjes die op de lijst verschijn is standaard 10, met een drop down menu voor verschillende hoeveelheden om op de pagina te tonen, dit doen we met het select element, vervolgens regelen met een onChange event listener het dat de pagina ververst wordt als deze veranderd wordt en dat er ook daadwerkelijk op dat moment 10, 25 of 50 items op de page geladen worden.</t>
+  </si>
+  <si>
+    <t>zoek pagina bevat een tekst input om daar de naam van het gewenste drankje te vinden.</t>
+  </si>
+  <si>
+    <t>is ook een button met een onSubmit functie welk eerder gedefinieerd is</t>
+  </si>
+  <si>
+    <t>find pagina heeft een radio button waarmee de gebruiker kan kiezen om of op ingrediënt of op naam van drankje te zoeken</t>
+  </si>
+  <si>
+    <t>functie van de onSubmit knop kijkt ten eerste of de contents van de zoekopdracht leeg staan, d.m.v. een if statement. Als dit ook leeg staat zet hij een andere variabele op true, deze variabele zal dan een popup op de pagina laten verschijnen, met een melding dat de zoekopdracht leeg was.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dit niet het geval is, wordt er met een else statement het volgende uitgevoerd. We maken variabele aan namens data en sturen binnen een try catch blok naar de backend een asynch axios GET request met de zoekopdracht</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> het catch blok een error opvangt maken we een alert aan dat er een fout is geweest met het halen van de data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> de request succesvol is wordt de data opgeslagen in ons data object.</t>
+  </si>
+  <si>
+    <t>volgens wordt er gekeken naar wat de response is, met een if/else statement renderen we nu een niks gevonden melding zou er niks gevonden zijn, alternatief kunnen we als allerlaatst in het de else statement de Showcase Page aanroepen met de data</t>
+  </si>
+  <si>
+    <t>kunnen een soortgelijke pagina als de showcase pagina aanroepen aangezien we ook een element willen tonen waar de gemaakte zoekopdracht terug te zien is, we kunnen dit of met properties voor de pagina maken waarmee we een component extra kunnen renderen of indien we gewoon een identieke pagina make met daarbij een  extra component.</t>
+  </si>
+  <si>
+    <t>Find pagina bevat een text input om daar de naam van het gewenste ingrediënt in te voeren.</t>
+  </si>
+  <si>
+    <t>elfde checks als bij zoeken op naam worden ook bij zoeken op ingrediënt uitgevoerd</t>
+  </si>
+  <si>
+    <t>gebruiker kan na het invullen van een query de resultaten op de preview items pagina zien, dit doet hij met behulp van een property die aan de pagina wordt mee gegeven, die de zoekopdracht in de GET request van de pagina zet, hiermee kan de gebruiker data doorgeven aan de GET voor de preview items pagina en zo wordt het alles doorgestuurd.</t>
+  </si>
+  <si>
+    <t>volgens worden alle items in de previewItems weergave op het scherm te zien.</t>
+  </si>
+  <si>
+    <t>de navigatiebalk is een Link naar de random item generator te vinden.</t>
+  </si>
+  <si>
+    <t>het moment dat de gebruiker op deze pagina beland is er in het midden een knop met een label get Random item. Deze knop heeft een onClick attribuut</t>
+  </si>
+  <si>
+    <t>is nogmaals een variabele namens data</t>
+  </si>
+  <si>
+    <t>random data wordt door middel van nog een asynchrone axios GET request binnen een try catch blok binnen gehaald vanuit de API backend en opgeslagen in het data object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> er een probleem is bij het binnenhalen van de data, dan toont het systeem een melding, met behulp van het catch blok.</t>
+  </si>
+  <si>
+    <t>het moment dat de data binnen gehaald is, wordt deze op de pagina weergegeven op de item preview modus</t>
+  </si>
+  <si>
+    <t>e item preview modus wordt in de standaard manier weergegeven, het enige verschil is dat deze keer een property meegegeven wordt voor de individuele preview pagina, gebaseerd op een conditie met behulp van een if statement, kunnen we de pagina op verschillende manieren renderen, zo kunnen we dezelfde PrevieItem pagina gebruiken, maar ook een knop hebben voor laatst getoonde drankje, dit betekent dat we nog steeds een Link naar die pagina kunnen behouden.</t>
+  </si>
+  <si>
+    <t>het laatste drankje weer te halen wat op de pagina te zien was slaan we deze met behulp van state op, op die manier kunnen we de laatst getoonde item nogmaals bekijken op het moment dat we erop drukken, als we met behulp van de lastItem variabele die met de setLastItem hook aangesproken wordt, weer dezelfde gegevens binnenhalen uit de lokale data en deze weer op het scherm weergeven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> er problemen zijn met requests naar de API kunnen we deze met behulp van try catch bloks en modals op de pagina weergeven zodat de gebruiker er iets aan kan doen</t>
+  </si>
+  <si>
+    <t>ruiker blijft van de ene pagina tot de ander m.b.v. de useContext hook ingelogd op het moment dat hij niet meer is ingelogd herleiden alle pagina’s naar de login page</t>
+  </si>
+  <si>
+    <t>e popups (bijvoorbeeld: security vraag bij het inloggen) ook modals genoemd, zullen met state te maken hebben, met verschillende routing zal de CSS en JSX van de popup met een if statement bepalen of deze true is, afhankelijk van de true waarde, of deze waar is of niet, zal of de ene versie van de pagina, of de andere geladen worden, op die manier zullen we op dezelfde pagina pop-ups en meerdere schermen kunnen laten gebeuren. en deze met een conditionele if statement voor de return statement gebruiken.</t>
+  </si>
+  <si>
+    <t>r middel van een onClick handler kan je een cocktail vergroten en zo de cocktail op een grotere manier op het scherm plaats laten nemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> je een cocktail je favoriet maakt wordt het id daarvan gepakt en doorgestuurd naar een lege array met favorieten die bij jouw account staat door middel van een methode die in het drankje component zit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> drankjes favoriet icon heeft verschillende styling, afhankelijk van of je het drankje al is eerder hebt toegevoegd aan favorieten of niet</t>
+  </si>
+  <si>
+    <t>het moment dat het drankje succesvol is opgeslagen in de backend wordt er een melding gedaan op het scherm waar het vermeld wordt dat deze succesvol is opgeslagen.</t>
   </si>
 </sst>
 </file>
@@ -132,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +319,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -182,80 +365,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -272,10 +393,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="719995"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -586,19 +707,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E3582-EACF-42CA-9681-43C1A515A0A2}">
   <dimension ref="B2:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="C19" zoomScale="154" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="9.109375" style="2"/>
-    <col min="3" max="3" width="174.21875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="174.28515625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -606,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -614,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -622,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -630,7 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -638,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -646,7 +767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>7</v>
       </c>
@@ -654,7 +775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -662,7 +783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>9</v>
       </c>
@@ -670,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>10</v>
       </c>
@@ -678,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>11</v>
       </c>
@@ -686,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>12</v>
       </c>
@@ -694,11 +815,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>13</v>
       </c>
@@ -706,7 +827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>14</v>
       </c>
@@ -714,7 +835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>15</v>
       </c>
@@ -722,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>16</v>
       </c>
@@ -730,7 +851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>17</v>
       </c>
@@ -738,7 +859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>18</v>
       </c>
@@ -746,7 +867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>19</v>
       </c>
@@ -754,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>20</v>
       </c>
@@ -762,7 +883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>21</v>
       </c>
@@ -770,7 +891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>22</v>
       </c>
@@ -778,10 +899,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>23</v>
       </c>
@@ -789,7 +910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>24</v>
       </c>
@@ -797,27 +918,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>29</v>
       </c>
@@ -829,15 +950,493 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487B4BC9-36A5-4D0C-8A09-89EAA770EEAB}">
-  <dimension ref="A1"/>
+  <dimension ref="C5:D63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="175.5703125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="4">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="4">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="4">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C13" s="4">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="4">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="4">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>15</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" s="4">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C22" s="4">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
+        <v>19</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
+        <v>20</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>21</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
+        <v>22</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
+        <v>23</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
+        <v>24</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="4">
+        <v>25</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="4">
+        <v>26</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="4">
+        <v>27</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C32" s="4">
+        <v>28</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="4">
+        <v>29</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="4">
+        <v>30</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C35" s="4">
+        <v>31</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="4">
+        <v>32</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="4">
+        <v>33</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="4">
+        <v>34</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="4">
+        <v>35</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C40" s="4">
+        <v>36</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="4">
+        <v>37</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="4">
+        <v>38</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C43" s="4">
+        <v>39</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C44" s="4">
+        <v>40</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="4">
+        <v>41</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="4">
+        <v>42</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C47" s="4">
+        <v>43</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="4">
+        <v>44</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="4">
+        <v>45</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="4">
+        <v>46</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="4">
+        <v>47</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="4">
+        <v>48</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="4">
+        <v>49</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="4">
+        <v>50</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C55" s="4">
+        <v>51</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C56" s="4">
+        <v>52</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="4">
+        <v>53</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="4">
+        <v>54</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C59" s="4">
+        <v>55</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="4">
+        <v>56</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C61" s="4">
+        <v>57</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="4">
+        <v>58</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="4">
+        <v>59</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Continued work on the requirements -2
</commit_message>
<xml_diff>
--- a/docs/Eisen.xlsx
+++ b/docs/Eisen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\WebstormProjects\fakeStore\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0F06C8-0841-4DCA-B4A1-8EA1B783F362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B26EF5-4B81-4634-8204-54EB00D18B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50FB539B-D8C3-40BF-ABB1-A5265842B59E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t xml:space="preserve">Een gebruiker moet kunnen registreren, dit kan op een registratie pagina, 
 deze is te vinden door te klikken op registreer vanuit de login pagina. </t>
@@ -112,48 +112,9 @@
     <t>Als er een fout is bij het halen van een request naar de backend, wordt dit aan de gebruiker doorgegeven.</t>
   </si>
   <si>
-    <t>Bij de registratie worden alle waardes aan de voorkant gecontroleerd met een if statement, als er een fout is waardoor de registratie niet voltooid kan worden, wordt er een melding gedaan, en wordt de gebruiker vervolgens terug naar het registreer scherm gestuurd met alle al ingevulde informatie.</t>
-  </si>
-  <si>
-    <t>Op het moment dat alle gebruikers gegevens correct zijn worden deze opgeslagen in een object en d.m.v. een Post request naar de backend estuurd, voortaan zal de gebruiker deze gegevens kunnen gebruiken om in te loggen</t>
-  </si>
-  <si>
     <t>Dit wordt met behulp van een try catch blok gedaan, deze zorgt ervoor dat er een melding verschijn als er iets misgaat.</t>
   </si>
   <si>
-    <t>Als alles ingevuld is wordt er met behulp van routes een link getoont op de pagina, deze herleidt naar de login pagina</t>
-  </si>
-  <si>
-    <t>Als een gebruiker niet is ingelogd, dit wordt standaard door context aangegeven, dan moet elke pagina de gebruiker naar de login pagina/register pagine terugleiden, dit doen we door middel van een login required page, deze pagina roepen we aan als een component bij elke pagina als authorized context op false staat, dit kunnen we door middel van een if statement op de pagina doen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Als een gebruiker gegevens invoert om in te loggen, worden deze met een POST request naar de backend gestuurd, afhankelijk daarvan krijgt de gebruiker een JSX-token, </t>
-  </si>
-  <si>
-    <t>De POST request wordt ook binnen een try catch blok geplaatst om op die manier errors die eruit komen te kunnen vermelden, op die manier kan de gebruiker kijken en reageren, stel voor zijn kat bijt de ethernet kabel door, dan weet hij wat het probleem is.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We slaan de JSX-token op met behulp van een asynchrone functie en state, in een variabele genoemd loginSuccess </t>
-  </si>
-  <si>
-    <t>Als de loginSuccess variabele truthy is dan wordt de gebruiker ingelogd. anders wordt er een melding in de vorm van een alert zichtbaar, dit is mogelijk met een if else statement. Als loginSucces truthy is dan loggen we de gebruiker met behulp van state en in, op alle andere pagina’s wordt de loginSuccess state met context binnengehaald om op die manier de gebruiker te autoriseren om door te kunnen gaan. Als de gebruiker faalt met het inloggen krijgen ze nogmaals de capaciteit om te proberen in te loggen op de login pagina</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> behulp van routing kunnen we op de navigatie balk een nav linken naar de profiel pagina als de gebruiker ingelogd is</t>
-  </si>
-  <si>
-    <t>data op de profiel pagina (mail, username, password) zal door middel van een Get request binnen een try catch blok gepakt worden om op de pagina getoont te worden</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> er een foto is geupload door de gebruiker, dan zal deze met een andere GET request binnen een try catch blok gehaald worden en op de pagina verschijnen. Als er een GET gemaakt wordt en het antwoord is leeg, dan gebruiken state om een variabele profilePictureIsEmpty op true te zetten</t>
-  </si>
-  <si>
-    <t>de Profiel Pagina zal er een knop zijn met een label, de label is gegevens bewerken. Op het moment dat de knop gedrukt wordt zal het een handleClick functie aanroepen. Deze zal een variabele bewerkingsmodus door middel van state aanpassen naar true.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> een input van type file zullen we een foto kunnen selecteren, vervolgens zullen we een asynchrone axios functie aan kunnen roepen met een onChange event listener. Op deze manier kunnen we een profielfoto uploaden</t>
-  </si>
-  <si>
     <t xml:space="preserve">Profiel Pagina is een pagina die voor de return statement een if statement heeft, daardoor zullen we met hulp van of de ene conditie of de andere de pagina op een andere manier kunnen laten zien, waar eerder de gegevens niet te bewerken waren, zal er nu door het feit dat de bewerkingsmodus variabele nu op true staat een andere versie van de pagina te zien zijn, aangezien er nu een andere return statement aangeroepen wordt. Dit betekent dat we de gegevens nu in een form kunnen zetten, met textvelden als inputs met bijbehorende labels. </t>
   </si>
   <si>
@@ -287,6 +248,36 @@
   </si>
   <si>
     <t>het moment dat het drankje succesvol is opgeslagen in de backend wordt er een melding gedaan op het scherm waar het vermeld wordt dat deze succesvol is opgeslagen.</t>
+  </si>
+  <si>
+    <t>Bij de registratie worden alle waardes aan de voorkant gecontroleerd, als er een fout is waardoor de registratie niet voltooid kan worden, wordt er een melding gedaan, en wordt de gebruiker vervolgens terug naar het registreer scherm gestuurd met alle alvast ingevulde informatie.</t>
+  </si>
+  <si>
+    <t>Op het moment dat alle gebruikers gegevens correct zijn worden deze opgeslagen in een object en d.m.v. een Post request naar de backend gestuurd, voortaan zal de gebruiker deze gegevens kunnen gebruiken om in te loggen</t>
+  </si>
+  <si>
+    <t>Als de gegevens succesvol geregistreerd zijn en het registratie proces afgerond is, wordt de gebruiker herleidt naar de home pagina</t>
+  </si>
+  <si>
+    <t>Als een gebruiker niet is ingelogd (dit wordt standaard door context aangegeven) dan moet elke pagina de gebruiker naar de login pagina/register pagina terugleiden, dit doen we door middel van een login required page, deze pagina roepen we aan als een component bij elke pagina als authorized context op false staat, dit kunnen we door middel van een if statement op de pagina doen.</t>
+  </si>
+  <si>
+    <t>Als een gebruiker gegevens invoert om in te loggen, worden deze met een POST request naar de backend gestuurd, afhankelijk daarvan krijgt de gebruiker een JSX-token, de JWT wordt in de local storage opgeslagen</t>
+  </si>
+  <si>
+    <t>De POST request wordt ook binnen een try catch blok geplaatst om op die manier errors die eruit komen te kunnen vermeiden, op die manier kan de gebruiker kijken en reageren, stel voor zijn kat bijt de ethernet kabel door, dan weet hij wat het probleem is.</t>
+  </si>
+  <si>
+    <t>m.b.v routing kunnen we op de navigatie balk een nav linken naar de profiel pagina als de gebruiker ingelogd is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user data zal d.m.v een GET request gehaald worden om op de profile pagina getoont te worden, </t>
+  </si>
+  <si>
+    <t>Op de Profiel Pagina zal er een knop zijn met tekst, de knop zal profiel gegevens bewerkingen ontgrendelen. Op het moment dat de knop gedrukt wordt zal het een handleClick functie aanroepen. Deze zal een variabele bewerkingsmodus door middel van state aanpassen naar true.</t>
+  </si>
+  <si>
+    <t>Ik wil een externe API inschakelen om adres suggesties te aanraden op basis van wat de gebruiker begint in te voeren bij zijn adres gegevens.</t>
   </si>
 </sst>
 </file>
@@ -356,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -370,6 +361,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E3582-EACF-42CA-9681-43C1A515A0A2}">
   <dimension ref="B2:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScale="154" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,228 +718,266 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+    </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+    </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+    </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+      <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="B16" s="4">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="B18" s="4">
         <v>13</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="4">
         <v>14</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="B20" s="4">
         <v>15</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+    </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+      <c r="B22" s="4">
         <v>16</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+      <c r="B23" s="4">
         <v>17</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+    </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+      <c r="B25" s="4">
         <v>18</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+    </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
+      <c r="B27" s="4">
         <v>19</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+    </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
+      <c r="B29" s="4">
         <v>20</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
+      <c r="B30" s="4">
         <v>21</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
+      <c r="B31" s="4">
         <v>22</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
+      <c r="B33" s="4">
         <v>23</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
+      <c r="B34" s="4">
         <v>24</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="5" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+    </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
+      <c r="B36" s="4">
         <v>25</v>
       </c>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
+      <c r="B37" s="4">
         <v>26</v>
       </c>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="2">
+      <c r="B38" s="4">
         <v>27</v>
       </c>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="2">
+      <c r="B39" s="4">
         <v>28</v>
       </c>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="2">
+      <c r="B40" s="4">
         <v>29</v>
       </c>
+      <c r="C40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -950,490 +986,492 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487B4BC9-36A5-4D0C-8A09-89EAA770EEAB}">
-  <dimension ref="C5:D63"/>
+  <dimension ref="C5:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="119" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="3" max="3" width="5.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="175.5703125" style="3" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
+      <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="7">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="7">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="7">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="7">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="7">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="7">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" s="7">
+        <v>15</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
+    <row r="22" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="7">
+        <v>16</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="4">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5" t="s">
+    <row r="23" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C23" s="7">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
+    <row r="24" spans="3:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C24" s="7">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="4">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
+    <row r="25" spans="3:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C25" s="7">
+        <v>19</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="4">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5" t="s">
+    <row r="26" spans="3:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C26" s="7">
+        <v>20</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="4">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5" t="s">
+    <row r="27" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="7">
+        <v>21</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C13" s="4">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="7">
+        <v>22</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="4">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5" t="s">
+    <row r="29" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="7">
+        <v>23</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="4">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="7">
+        <v>24</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="4">
-        <v>12</v>
-      </c>
-      <c r="D16" s="5" t="s">
+    <row r="31" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="7">
+        <v>25</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C17" s="4">
-        <v>13</v>
-      </c>
-      <c r="D17" s="5" t="s">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="7">
+        <v>26</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="4">
-        <v>14</v>
-      </c>
-      <c r="D18" s="5" t="s">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="7">
+        <v>27</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="4">
-        <v>15</v>
-      </c>
-      <c r="D19" s="5" t="s">
+    <row r="34" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C34" s="7">
+        <v>28</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="4">
-        <v>16</v>
-      </c>
-      <c r="D20" s="5" t="s">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="7">
+        <v>29</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C21" s="4">
-        <v>17</v>
-      </c>
-      <c r="D21" s="5" t="s">
+    <row r="36" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="7">
+        <v>30</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C22" s="4">
-        <v>18</v>
-      </c>
-      <c r="D22" s="5" t="s">
+    <row r="37" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C37" s="7">
+        <v>31</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="3:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C23" s="4">
-        <v>19</v>
-      </c>
-      <c r="D23" s="5" t="s">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="7">
+        <v>32</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C24" s="4">
-        <v>20</v>
-      </c>
-      <c r="D24" s="5" t="s">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="7">
+        <v>33</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="4">
-        <v>21</v>
-      </c>
-      <c r="D25" s="5" t="s">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="7">
+        <v>34</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="4">
-        <v>22</v>
-      </c>
-      <c r="D26" s="5" t="s">
+    <row r="41" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C41" s="7">
+        <v>35</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="4">
-        <v>23</v>
-      </c>
-      <c r="D27" s="5" t="s">
+    <row r="42" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="7">
+        <v>36</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="4">
-        <v>24</v>
-      </c>
-      <c r="D28" s="5" t="s">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="7">
+        <v>37</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C29" s="4">
-        <v>25</v>
-      </c>
-      <c r="D29" s="5" t="s">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="7">
+        <v>38</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="4">
-        <v>26</v>
-      </c>
-      <c r="D30" s="5" t="s">
+    <row r="45" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C45" s="7">
+        <v>39</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="4">
-        <v>27</v>
-      </c>
-      <c r="D31" s="5" t="s">
+    <row r="46" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C46" s="7">
+        <v>40</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C32" s="4">
-        <v>28</v>
-      </c>
-      <c r="D32" s="5" t="s">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="7">
+        <v>41</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="4">
-        <v>29</v>
-      </c>
-      <c r="D33" s="5" t="s">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="7">
+        <v>42</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C34" s="4">
-        <v>30</v>
-      </c>
-      <c r="D34" s="5" t="s">
+    <row r="49" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C49" s="7">
+        <v>43</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C35" s="4">
-        <v>31</v>
-      </c>
-      <c r="D35" s="5" t="s">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="7">
+        <v>44</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="4">
-        <v>32</v>
-      </c>
-      <c r="D36" s="5" t="s">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="7">
+        <v>45</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="4">
-        <v>33</v>
-      </c>
-      <c r="D37" s="5" t="s">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="7">
+        <v>46</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="4">
-        <v>34</v>
-      </c>
-      <c r="D38" s="5" t="s">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="7">
+        <v>47</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C39" s="4">
-        <v>35</v>
-      </c>
-      <c r="D39" s="5" t="s">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="7">
+        <v>48</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C40" s="4">
-        <v>36</v>
-      </c>
-      <c r="D40" s="5" t="s">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="7">
+        <v>49</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="4">
-        <v>37</v>
-      </c>
-      <c r="D41" s="5" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="7">
+        <v>50</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="4">
-        <v>38</v>
-      </c>
-      <c r="D42" s="5" t="s">
+    <row r="57" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C57" s="7">
+        <v>51</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C43" s="4">
-        <v>39</v>
-      </c>
-      <c r="D43" s="5" t="s">
+    <row r="58" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C58" s="7">
+        <v>52</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C44" s="4">
-        <v>40</v>
-      </c>
-      <c r="D44" s="5" t="s">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="7">
+        <v>53</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="4">
-        <v>41</v>
-      </c>
-      <c r="D45" s="5" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="7">
+        <v>54</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="4">
-        <v>42</v>
-      </c>
-      <c r="D46" s="5" t="s">
+    <row r="61" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C61" s="7">
+        <v>55</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C47" s="4">
-        <v>43</v>
-      </c>
-      <c r="D47" s="5" t="s">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="7">
+        <v>56</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="4">
-        <v>44</v>
-      </c>
-      <c r="D48" s="5" t="s">
+    <row r="63" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C63" s="7">
+        <v>57</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="4">
-        <v>45</v>
-      </c>
-      <c r="D49" s="5" t="s">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="7">
+        <v>58</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="4">
-        <v>46</v>
-      </c>
-      <c r="D50" s="5" t="s">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="7">
+        <v>59</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="4">
-        <v>47</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="4">
-        <v>48</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="4">
-        <v>49</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="4">
-        <v>50</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C55" s="4">
-        <v>51</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C56" s="4">
-        <v>52</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="4">
-        <v>53</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="4">
-        <v>54</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C59" s="4">
-        <v>55</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="4">
-        <v>56</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C61" s="4">
-        <v>57</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="4">
-        <v>58</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="4">
-        <v>59</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>